<commit_message>
Adding some domain changes
</commit_message>
<xml_diff>
--- a/techdebtscore-model.xlsx
+++ b/techdebtscore-model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhurff/projects/jhurff/allninjas/tools/allninjas-techdebtscore/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhurff/projects/jhurff/smartbrains/tools/smartbrains-techdebtscore/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C916AD6-4AC2-7748-AC5F-C3491A8A6C12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D08C4D36-2F39-1240-8B07-D1ABB54B6234}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="460" windowWidth="28120" windowHeight="16660" xr2:uid="{8CB8C874-9271-7F42-B933-94FB11224F90}"/>
+    <workbookView xWindow="900" yWindow="2140" windowWidth="28120" windowHeight="16660" activeTab="4" xr2:uid="{8CB8C874-9271-7F42-B933-94FB11224F90}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -1978,7 +1978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18C4BD8E-A134-7041-9B07-8B6F1CECF9F4}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+    <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
       <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
@@ -2363,15 +2363,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47D104A9-DB65-4A47-B132-051F6731D23D}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" customWidth="1"/>
-    <col min="5" max="6" width="14" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="4" max="5" width="16.83203125" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
     <col min="8" max="8" width="13.6640625" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
   </cols>

</xml_diff>